<commit_message>
Fixes RF_B_Sel signal on immediate instructions
</commit_message>
<xml_diff>
--- a/Control_signals.xlsx
+++ b/Control_signals.xlsx
@@ -181,7 +181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -196,6 +196,11 @@
     <font>
       <name val="Calibri"/>
       <color theme="1" tint="0"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
@@ -291,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -345,6 +350,9 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="3" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -354,13 +362,7 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="5" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1766,8 +1768,8 @@
       <c r="G23" s="3">
         <v>0</v>
       </c>
-      <c r="H23" s="3">
-        <v>0</v>
+      <c r="H23" s="19">
+        <v>1</v>
       </c>
       <c r="I23" s="3">
         <v>0</v>
@@ -1814,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="3">
         <v>0</v>
@@ -1861,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="8">
         <v>0</v>
@@ -1907,7 +1909,7 @@
       <c r="G26" s="3">
         <v>0</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="10">
         <v>0</v>
       </c>
       <c r="I26" s="3">
@@ -1981,8 +1983,8 @@
       <c r="G28" s="3">
         <v>0</v>
       </c>
-      <c r="H28" s="3">
-        <v>0</v>
+      <c r="H28" s="19">
+        <v>1</v>
       </c>
       <c r="I28" s="3">
         <v>0</v>
@@ -2029,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="3">
         <v>0</v>
@@ -2076,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="8">
         <v>0</v>
@@ -2122,7 +2124,7 @@
       <c r="G31" s="3">
         <v>0</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="10">
         <v>0</v>
       </c>
       <c r="I31" s="3">
@@ -2196,8 +2198,8 @@
       <c r="G33" s="3">
         <v>0</v>
       </c>
-      <c r="H33" s="8">
-        <v>0</v>
+      <c r="H33" s="19">
+        <v>1</v>
       </c>
       <c r="I33" s="3">
         <v>0</v>
@@ -2244,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="3">
         <v>0</v>
@@ -2291,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="8">
         <v>0</v>
@@ -2337,7 +2339,7 @@
       <c r="G36" s="3">
         <v>0</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="10">
         <v>0</v>
       </c>
       <c r="I36" s="3">
@@ -2411,8 +2413,8 @@
       <c r="G38" s="3">
         <v>0</v>
       </c>
-      <c r="H38" s="8">
-        <v>0</v>
+      <c r="H38" s="19">
+        <v>1</v>
       </c>
       <c r="I38" s="3">
         <v>0</v>
@@ -2459,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="3">
         <v>0</v>
@@ -2506,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="8">
         <v>0</v>
@@ -2517,7 +2519,7 @@
       <c r="K40" s="6">
         <v>1</v>
       </c>
-      <c r="L40" s="19" t="s">
+      <c r="L40" s="20" t="s">
         <v>15</v>
       </c>
       <c r="M40" s="3">
@@ -2552,7 +2554,7 @@
       <c r="G41" s="3">
         <v>0</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="10">
         <v>0</v>
       </c>
       <c r="I41" s="3">
@@ -2626,8 +2628,8 @@
       <c r="G43" s="3">
         <v>0</v>
       </c>
-      <c r="H43" s="8">
-        <v>0</v>
+      <c r="H43" s="19">
+        <v>1</v>
       </c>
       <c r="I43" s="3">
         <v>0</v>
@@ -2674,7 +2676,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="3">
         <v>0</v>
@@ -2721,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="H45" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="8">
         <v>0</v>
@@ -2732,7 +2734,7 @@
       <c r="K45" s="6">
         <v>1</v>
       </c>
-      <c r="L45" s="19" t="s">
+      <c r="L45" s="20" t="s">
         <v>15</v>
       </c>
       <c r="M45" s="3">
@@ -2767,7 +2769,7 @@
       <c r="G46" s="3">
         <v>0</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="10">
         <v>0</v>
       </c>
       <c r="I46" s="3">
@@ -2841,8 +2843,8 @@
       <c r="G49" s="3">
         <v>0</v>
       </c>
-      <c r="H49" s="3">
-        <v>0</v>
+      <c r="H49" s="19">
+        <v>1</v>
       </c>
       <c r="I49" s="3">
         <v>0</v>
@@ -2882,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="3">
         <v>0</v>
@@ -2922,7 +2924,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="3">
         <v>0</v>
@@ -2961,7 +2963,7 @@
       <c r="G52" s="3">
         <v>0</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="10">
         <v>0</v>
       </c>
       <c r="I52" s="3">
@@ -3072,7 +3074,7 @@
       <c r="K55" s="6">
         <v>0</v>
       </c>
-      <c r="L55" s="20" t="s">
+      <c r="L55" s="21" t="s">
         <v>15</v>
       </c>
       <c r="M55" s="3">
@@ -3140,8 +3142,8 @@
       <c r="G57" s="3">
         <v>0</v>
       </c>
-      <c r="H57" s="6">
-        <v>1</v>
+      <c r="H57" s="10">
+        <v>0</v>
       </c>
       <c r="I57" s="3">
         <v>0</v>
@@ -3251,7 +3253,7 @@
       <c r="K60" s="6">
         <v>0</v>
       </c>
-      <c r="L60" s="20" t="s">
+      <c r="L60" s="21" t="s">
         <v>15</v>
       </c>
       <c r="M60" s="3">
@@ -3319,8 +3321,8 @@
       <c r="G62" s="3">
         <v>0</v>
       </c>
-      <c r="H62" s="6">
-        <v>1</v>
+      <c r="H62" s="10">
+        <v>0</v>
       </c>
       <c r="I62" s="3">
         <v>0</v>
@@ -3353,7 +3355,7 @@
       <c r="I63" s="18"/>
       <c r="J63" s="18"/>
       <c r="K63" s="18"/>
-      <c r="L63" s="21"/>
+      <c r="L63" s="22"/>
       <c r="M63" s="2"/>
     </row>
     <row r="64" ht="14.25">
@@ -3368,7 +3370,7 @@
       <c r="I64" s="18"/>
       <c r="J64" s="18"/>
       <c r="K64" s="18"/>
-      <c r="L64" s="21"/>
+      <c r="L64" s="22"/>
       <c r="M64" s="2"/>
     </row>
     <row r="65" ht="14.25">
@@ -3383,7 +3385,7 @@
       <c r="I65" s="18"/>
       <c r="J65" s="18"/>
       <c r="K65" s="18"/>
-      <c r="L65" s="21"/>
+      <c r="L65" s="22"/>
       <c r="M65" s="2"/>
     </row>
     <row r="66" ht="14.25">
@@ -3398,7 +3400,7 @@
       <c r="I66" s="18"/>
       <c r="J66" s="18"/>
       <c r="K66" s="18"/>
-      <c r="L66" s="21"/>
+      <c r="L66" s="22"/>
       <c r="M66" s="2"/>
     </row>
     <row r="67" ht="14.25">
@@ -3420,7 +3422,7 @@
       <c r="A68" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="B68" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C68" s="4" t="s">
@@ -3438,8 +3440,8 @@
       <c r="G68" s="3">
         <v>0</v>
       </c>
-      <c r="H68" s="3">
-        <v>0</v>
+      <c r="H68" s="19">
+        <v>1</v>
       </c>
       <c r="I68" s="3">
         <v>0</v>
@@ -3479,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="H69" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69" s="3">
         <v>0</v>
@@ -3519,7 +3521,7 @@
         <v>0</v>
       </c>
       <c r="H70" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" s="3">
         <v>0</v>
@@ -3559,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="H71" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" s="8">
         <v>1</v>
@@ -3598,7 +3600,7 @@
       <c r="G72" s="3">
         <v>0</v>
       </c>
-      <c r="H72" s="3">
+      <c r="H72" s="10">
         <v>0</v>
       </c>
       <c r="I72" s="10">
@@ -3657,8 +3659,8 @@
       <c r="G74" s="3">
         <v>0</v>
       </c>
-      <c r="H74" s="6">
-        <v>0</v>
+      <c r="H74" s="8">
+        <v>1</v>
       </c>
       <c r="I74" s="3">
         <v>0</v>
@@ -3697,7 +3699,7 @@
       <c r="G75" s="3">
         <v>0</v>
       </c>
-      <c r="H75" s="8">
+      <c r="H75" s="6">
         <v>1</v>
       </c>
       <c r="I75" s="3">
@@ -3765,7 +3767,7 @@
       <c r="C77" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D77" s="20" t="s">
+      <c r="D77" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E77" s="8">
@@ -3804,10 +3806,10 @@
       <c r="B78" s="7"/>
     </row>
     <row r="79" ht="14.25">
-      <c r="A79" s="24" t="s">
+      <c r="A79" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C79" s="4" t="s">
@@ -3825,8 +3827,8 @@
       <c r="G79" s="3">
         <v>0</v>
       </c>
-      <c r="H79" s="3">
-        <v>0</v>
+      <c r="H79" s="19">
+        <v>1</v>
       </c>
       <c r="I79" s="3">
         <v>0</v>
@@ -3866,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="H80" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I80" s="3">
         <v>0</v>
@@ -3906,7 +3908,7 @@
         <v>0</v>
       </c>
       <c r="H81" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81" s="3">
         <v>0</v>
@@ -3946,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="H82" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I82" s="8">
         <v>1</v>
@@ -3985,7 +3987,7 @@
       <c r="G83" s="3">
         <v>0</v>
       </c>
-      <c r="H83" s="3">
+      <c r="H83" s="10">
         <v>0</v>
       </c>
       <c r="I83" s="10">
@@ -4023,10 +4025,10 @@
       <c r="M84" s="2"/>
     </row>
     <row r="85" ht="14.25">
-      <c r="A85" s="24" t="s">
+      <c r="A85" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -4044,8 +4046,8 @@
       <c r="G85" s="3">
         <v>0</v>
       </c>
-      <c r="H85" s="6">
-        <v>0</v>
+      <c r="H85" s="8">
+        <v>1</v>
       </c>
       <c r="I85" s="3">
         <v>0</v>
@@ -4084,7 +4086,7 @@
       <c r="G86" s="3">
         <v>0</v>
       </c>
-      <c r="H86" s="8">
+      <c r="H86" s="6">
         <v>1</v>
       </c>
       <c r="I86" s="3">
@@ -4152,7 +4154,7 @@
       <c r="C88" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D88" s="20" t="s">
+      <c r="D88" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E88" s="8">

</xml_diff>